<commit_message>
Some fixes in the excel templates/narvarokort.xlsx template
</commit_message>
<xml_diff>
--- a/templates/narvarokort.xlsx
+++ b/templates/narvarokort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\skojjt\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD2D11B-4725-4FFD-917A-150E83F94BE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0FB8E5-EFDE-41BB-B272-5B3578D73023}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32772" yWindow="32772" windowWidth="30720" windowHeight="13368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,8 +1134,6 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
@@ -1145,12 +1143,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
@@ -1172,10 +1168,12 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1184,6 +1182,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2120,7 +2124,7 @@
   <dimension ref="A1:AZ44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2144,14 +2148,14 @@
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
       <c r="D1" s="56"/>
-      <c r="E1" s="126" t="s">
+      <c r="E1" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="127"/>
-      <c r="G1" s="129" t="s">
+      <c r="F1" s="125"/>
+      <c r="G1" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="129"/>
+      <c r="H1" s="127"/>
       <c r="I1" s="57" t="s">
         <v>69</v>
       </c>
@@ -2264,7 +2268,7 @@
       <c r="AT1" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="AU1" s="130"/>
+      <c r="AU1" s="119"/>
       <c r="AV1" s="56"/>
       <c r="AW1" s="56"/>
       <c r="AX1" s="27"/>
@@ -2283,46 +2287,46 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="128" t="s">
+      <c r="J2" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="123"/>
-      <c r="O2" s="123"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="123"/>
-      <c r="S2" s="123"/>
-      <c r="T2" s="123"/>
-      <c r="U2" s="123"/>
-      <c r="V2" s="123"/>
-      <c r="W2" s="123"/>
-      <c r="X2" s="123"/>
-      <c r="Y2" s="123"/>
-      <c r="Z2" s="123"/>
-      <c r="AA2" s="123"/>
-      <c r="AB2" s="123"/>
-      <c r="AC2" s="123"/>
-      <c r="AD2" s="123"/>
-      <c r="AE2" s="123"/>
-      <c r="AF2" s="123"/>
-      <c r="AG2" s="123"/>
-      <c r="AH2" s="123"/>
-      <c r="AI2" s="123"/>
-      <c r="AJ2" s="123"/>
-      <c r="AK2" s="123"/>
-      <c r="AL2" s="123"/>
-      <c r="AM2" s="123"/>
-      <c r="AN2" s="123"/>
-      <c r="AO2" s="123"/>
-      <c r="AP2" s="123"/>
-      <c r="AQ2" s="123"/>
-      <c r="AR2" s="123"/>
-      <c r="AS2" s="123"/>
-      <c r="AT2" s="123"/>
-      <c r="AU2" s="131" t="s">
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="121"/>
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="121"/>
+      <c r="AH2" s="121"/>
+      <c r="AI2" s="121"/>
+      <c r="AJ2" s="121"/>
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121"/>
+      <c r="AN2" s="121"/>
+      <c r="AO2" s="121"/>
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="121"/>
+      <c r="AT2" s="121"/>
+      <c r="AU2" s="120" t="s">
         <v>71</v>
       </c>
       <c r="AX2" s="28"/>
@@ -2341,49 +2345,49 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="124"/>
-      <c r="O3" s="124"/>
-      <c r="P3" s="124"/>
-      <c r="Q3" s="124"/>
-      <c r="R3" s="124"/>
-      <c r="S3" s="124"/>
-      <c r="T3" s="124"/>
-      <c r="U3" s="124"/>
-      <c r="V3" s="124"/>
-      <c r="W3" s="124"/>
-      <c r="X3" s="124"/>
-      <c r="Y3" s="124"/>
-      <c r="Z3" s="124"/>
-      <c r="AA3" s="124"/>
-      <c r="AB3" s="124"/>
-      <c r="AC3" s="124"/>
-      <c r="AD3" s="124"/>
-      <c r="AE3" s="124"/>
-      <c r="AF3" s="124"/>
-      <c r="AG3" s="124"/>
-      <c r="AH3" s="124"/>
-      <c r="AI3" s="124"/>
-      <c r="AJ3" s="124"/>
-      <c r="AK3" s="124"/>
-      <c r="AL3" s="124"/>
-      <c r="AM3" s="124"/>
-      <c r="AN3" s="124"/>
-      <c r="AO3" s="124"/>
-      <c r="AP3" s="124"/>
-      <c r="AQ3" s="124"/>
-      <c r="AR3" s="124"/>
-      <c r="AS3" s="124"/>
-      <c r="AT3" s="124"/>
-      <c r="AU3" s="132" t="s">
+      <c r="J3" s="126"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="122"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="122"/>
+      <c r="S3" s="122"/>
+      <c r="T3" s="122"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="122"/>
+      <c r="X3" s="122"/>
+      <c r="Y3" s="122"/>
+      <c r="Z3" s="122"/>
+      <c r="AA3" s="122"/>
+      <c r="AB3" s="122"/>
+      <c r="AC3" s="122"/>
+      <c r="AD3" s="122"/>
+      <c r="AE3" s="122"/>
+      <c r="AF3" s="122"/>
+      <c r="AG3" s="122"/>
+      <c r="AH3" s="122"/>
+      <c r="AI3" s="122"/>
+      <c r="AJ3" s="122"/>
+      <c r="AK3" s="122"/>
+      <c r="AL3" s="122"/>
+      <c r="AM3" s="122"/>
+      <c r="AN3" s="122"/>
+      <c r="AO3" s="122"/>
+      <c r="AP3" s="122"/>
+      <c r="AQ3" s="122"/>
+      <c r="AR3" s="122"/>
+      <c r="AS3" s="122"/>
+      <c r="AT3" s="122"/>
+      <c r="AU3" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="AV3" s="133"/>
-      <c r="AW3" s="133"/>
-      <c r="AX3" s="134"/>
+      <c r="AV3" s="131"/>
+      <c r="AW3" s="131"/>
+      <c r="AX3" s="132"/>
     </row>
     <row r="4" spans="1:52" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
@@ -2399,85 +2403,85 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="124"/>
-      <c r="Y4" s="124"/>
-      <c r="Z4" s="124"/>
-      <c r="AA4" s="124"/>
-      <c r="AB4" s="124"/>
-      <c r="AC4" s="124"/>
-      <c r="AD4" s="124"/>
-      <c r="AE4" s="124"/>
-      <c r="AF4" s="124"/>
-      <c r="AG4" s="124"/>
-      <c r="AH4" s="124"/>
-      <c r="AI4" s="124"/>
-      <c r="AJ4" s="124"/>
-      <c r="AK4" s="124"/>
-      <c r="AL4" s="124"/>
-      <c r="AM4" s="124"/>
-      <c r="AN4" s="124"/>
-      <c r="AO4" s="124"/>
-      <c r="AP4" s="124"/>
-      <c r="AQ4" s="124"/>
-      <c r="AR4" s="124"/>
-      <c r="AS4" s="124"/>
-      <c r="AT4" s="124"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+      <c r="N4" s="122"/>
+      <c r="O4" s="122"/>
+      <c r="P4" s="122"/>
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="122"/>
+      <c r="W4" s="122"/>
+      <c r="X4" s="122"/>
+      <c r="Y4" s="122"/>
+      <c r="Z4" s="122"/>
+      <c r="AA4" s="122"/>
+      <c r="AB4" s="122"/>
+      <c r="AC4" s="122"/>
+      <c r="AD4" s="122"/>
+      <c r="AE4" s="122"/>
+      <c r="AF4" s="122"/>
+      <c r="AG4" s="122"/>
+      <c r="AH4" s="122"/>
+      <c r="AI4" s="122"/>
+      <c r="AJ4" s="122"/>
+      <c r="AK4" s="122"/>
+      <c r="AL4" s="122"/>
+      <c r="AM4" s="122"/>
+      <c r="AN4" s="122"/>
+      <c r="AO4" s="122"/>
+      <c r="AP4" s="122"/>
+      <c r="AQ4" s="122"/>
+      <c r="AR4" s="122"/>
+      <c r="AS4" s="122"/>
+      <c r="AT4" s="122"/>
       <c r="AU4" s="21"/>
       <c r="AX4" s="28"/>
     </row>
     <row r="5" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="124"/>
-      <c r="T5" s="124"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
-      <c r="Y5" s="124"/>
-      <c r="Z5" s="124"/>
-      <c r="AA5" s="124"/>
-      <c r="AB5" s="124"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="124"/>
-      <c r="AE5" s="124"/>
-      <c r="AF5" s="124"/>
-      <c r="AG5" s="124"/>
-      <c r="AH5" s="124"/>
-      <c r="AI5" s="124"/>
-      <c r="AJ5" s="124"/>
-      <c r="AK5" s="124"/>
-      <c r="AL5" s="124"/>
-      <c r="AM5" s="124"/>
-      <c r="AN5" s="124"/>
-      <c r="AO5" s="124"/>
-      <c r="AP5" s="124"/>
-      <c r="AQ5" s="124"/>
-      <c r="AR5" s="124"/>
-      <c r="AS5" s="124"/>
-      <c r="AT5" s="124"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="122"/>
+      <c r="N5" s="122"/>
+      <c r="O5" s="122"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="122"/>
+      <c r="S5" s="122"/>
+      <c r="T5" s="122"/>
+      <c r="U5" s="122"/>
+      <c r="V5" s="122"/>
+      <c r="W5" s="122"/>
+      <c r="X5" s="122"/>
+      <c r="Y5" s="122"/>
+      <c r="Z5" s="122"/>
+      <c r="AA5" s="122"/>
+      <c r="AB5" s="122"/>
+      <c r="AC5" s="122"/>
+      <c r="AD5" s="122"/>
+      <c r="AE5" s="122"/>
+      <c r="AF5" s="122"/>
+      <c r="AG5" s="122"/>
+      <c r="AH5" s="122"/>
+      <c r="AI5" s="122"/>
+      <c r="AJ5" s="122"/>
+      <c r="AK5" s="122"/>
+      <c r="AL5" s="122"/>
+      <c r="AM5" s="122"/>
+      <c r="AN5" s="122"/>
+      <c r="AO5" s="122"/>
+      <c r="AP5" s="122"/>
+      <c r="AQ5" s="122"/>
+      <c r="AR5" s="122"/>
+      <c r="AS5" s="122"/>
+      <c r="AT5" s="122"/>
       <c r="AU5" s="21"/>
       <c r="AV5" s="114"/>
       <c r="AX5" s="26"/>
@@ -2488,43 +2492,43 @@
       <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="128"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="125"/>
-      <c r="M6" s="125"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="125"/>
-      <c r="P6" s="125"/>
-      <c r="Q6" s="125"/>
-      <c r="R6" s="125"/>
-      <c r="S6" s="125"/>
-      <c r="T6" s="125"/>
-      <c r="U6" s="125"/>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="125"/>
-      <c r="Z6" s="125"/>
-      <c r="AA6" s="125"/>
-      <c r="AB6" s="125"/>
-      <c r="AC6" s="125"/>
-      <c r="AD6" s="125"/>
-      <c r="AE6" s="125"/>
-      <c r="AF6" s="125"/>
-      <c r="AG6" s="125"/>
-      <c r="AH6" s="125"/>
-      <c r="AI6" s="125"/>
-      <c r="AJ6" s="125"/>
-      <c r="AK6" s="125"/>
-      <c r="AL6" s="125"/>
-      <c r="AM6" s="125"/>
-      <c r="AN6" s="125"/>
-      <c r="AO6" s="125"/>
-      <c r="AP6" s="125"/>
-      <c r="AQ6" s="125"/>
-      <c r="AR6" s="125"/>
-      <c r="AS6" s="125"/>
-      <c r="AT6" s="125"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="123"/>
+      <c r="O6" s="123"/>
+      <c r="P6" s="123"/>
+      <c r="Q6" s="123"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
+      <c r="T6" s="123"/>
+      <c r="U6" s="123"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="123"/>
+      <c r="AC6" s="123"/>
+      <c r="AD6" s="123"/>
+      <c r="AE6" s="123"/>
+      <c r="AF6" s="123"/>
+      <c r="AG6" s="123"/>
+      <c r="AH6" s="123"/>
+      <c r="AI6" s="123"/>
+      <c r="AJ6" s="123"/>
+      <c r="AK6" s="123"/>
+      <c r="AL6" s="123"/>
+      <c r="AM6" s="123"/>
+      <c r="AN6" s="123"/>
+      <c r="AO6" s="123"/>
+      <c r="AP6" s="123"/>
+      <c r="AQ6" s="123"/>
+      <c r="AR6" s="123"/>
+      <c r="AS6" s="123"/>
+      <c r="AT6" s="123"/>
       <c r="AU6" s="21"/>
       <c r="AX6" s="26"/>
     </row>
@@ -2914,10 +2918,10 @@
       <c r="AT12" s="76"/>
       <c r="AU12" s="77"/>
       <c r="AV12" s="77"/>
-      <c r="AW12" s="121" t="s">
+      <c r="AW12" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="AX12" s="122"/>
+      <c r="AX12" s="129"/>
     </row>
     <row r="13" spans="1:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="82" t="s">
@@ -4595,7 +4599,7 @@
       <c r="C41" s="40"/>
       <c r="D41" s="41"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="116">
+      <c r="F41" s="134">
         <f>COUNTIFS(K2:AT6,"&lt;&gt;"&amp;"")</f>
         <v>0</v>
       </c>
@@ -4605,138 +4609,147 @@
       <c r="J41" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K41" s="118">
+      <c r="K41" s="116">
         <f>SUM(K13:K40)</f>
         <v>0</v>
       </c>
-      <c r="L41" s="118">
+      <c r="L41" s="116">
         <f t="shared" ref="L41:AT41" si="2">SUM(L13:L40)</f>
         <v>0</v>
       </c>
-      <c r="M41" s="118">
+      <c r="M41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N41" s="118">
+      <c r="N41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O41" s="118">
+      <c r="O41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P41" s="118">
+      <c r="P41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="118">
+      <c r="Q41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R41" s="118">
+      <c r="R41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S41" s="118">
+      <c r="S41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T41" s="118">
+      <c r="T41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U41" s="118">
+      <c r="U41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V41" s="118">
+      <c r="V41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W41" s="118">
+      <c r="W41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X41" s="118">
+      <c r="X41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y41" s="118">
+      <c r="Y41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z41" s="118">
+      <c r="Z41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA41" s="118">
+      <c r="AA41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB41" s="118">
+      <c r="AB41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC41" s="118">
+      <c r="AC41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD41" s="118">
+      <c r="AD41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE41" s="118">
+      <c r="AE41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF41" s="118">
+      <c r="AF41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG41" s="118">
+      <c r="AG41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH41" s="118"/>
-      <c r="AI41" s="118"/>
-      <c r="AJ41" s="118"/>
-      <c r="AK41" s="118">
+      <c r="AH41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AL41" s="118">
+      <c r="AI41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AM41" s="118">
+      <c r="AJ41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN41" s="118">
+      <c r="AK41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO41" s="118">
+      <c r="AL41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AP41" s="118">
+      <c r="AM41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AQ41" s="118">
+      <c r="AN41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AR41" s="118">
+      <c r="AO41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AS41" s="118">
+      <c r="AP41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AT41" s="118">
+      <c r="AQ41" s="116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AR41" s="116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AS41" s="116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AT41" s="116">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4768,42 +4781,42 @@
       <c r="J42" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K42" s="119"/>
-      <c r="L42" s="119"/>
-      <c r="M42" s="119"/>
-      <c r="N42" s="119"/>
-      <c r="O42" s="119"/>
-      <c r="P42" s="119"/>
-      <c r="Q42" s="119"/>
-      <c r="R42" s="119"/>
-      <c r="S42" s="119"/>
-      <c r="T42" s="119"/>
-      <c r="U42" s="119"/>
-      <c r="V42" s="119"/>
-      <c r="W42" s="119"/>
-      <c r="X42" s="119"/>
-      <c r="Y42" s="119"/>
-      <c r="Z42" s="119"/>
-      <c r="AA42" s="119"/>
-      <c r="AB42" s="119"/>
-      <c r="AC42" s="119"/>
-      <c r="AD42" s="119"/>
-      <c r="AE42" s="119"/>
-      <c r="AF42" s="119"/>
-      <c r="AG42" s="119"/>
-      <c r="AH42" s="119"/>
-      <c r="AI42" s="119"/>
-      <c r="AJ42" s="119"/>
-      <c r="AK42" s="119"/>
-      <c r="AL42" s="119"/>
-      <c r="AM42" s="119"/>
-      <c r="AN42" s="119"/>
-      <c r="AO42" s="119"/>
-      <c r="AP42" s="119"/>
-      <c r="AQ42" s="119"/>
-      <c r="AR42" s="119"/>
-      <c r="AS42" s="119"/>
-      <c r="AT42" s="119"/>
+      <c r="K42" s="117"/>
+      <c r="L42" s="117"/>
+      <c r="M42" s="117"/>
+      <c r="N42" s="117"/>
+      <c r="O42" s="117"/>
+      <c r="P42" s="117"/>
+      <c r="Q42" s="117"/>
+      <c r="R42" s="117"/>
+      <c r="S42" s="117"/>
+      <c r="T42" s="117"/>
+      <c r="U42" s="117"/>
+      <c r="V42" s="117"/>
+      <c r="W42" s="117"/>
+      <c r="X42" s="117"/>
+      <c r="Y42" s="117"/>
+      <c r="Z42" s="117"/>
+      <c r="AA42" s="117"/>
+      <c r="AB42" s="117"/>
+      <c r="AC42" s="117"/>
+      <c r="AD42" s="117"/>
+      <c r="AE42" s="117"/>
+      <c r="AF42" s="117"/>
+      <c r="AG42" s="117"/>
+      <c r="AH42" s="117"/>
+      <c r="AI42" s="117"/>
+      <c r="AJ42" s="117"/>
+      <c r="AK42" s="117"/>
+      <c r="AL42" s="117"/>
+      <c r="AM42" s="117"/>
+      <c r="AN42" s="117"/>
+      <c r="AO42" s="117"/>
+      <c r="AP42" s="117"/>
+      <c r="AQ42" s="117"/>
+      <c r="AR42" s="117"/>
+      <c r="AS42" s="117"/>
+      <c r="AT42" s="117"/>
       <c r="AU42" s="110"/>
       <c r="AV42" s="110"/>
       <c r="AW42" s="101"/>
@@ -4817,7 +4830,7 @@
       <c r="C43" s="52"/>
       <c r="D43" s="52"/>
       <c r="E43" s="37"/>
-      <c r="F43" s="117">
+      <c r="F43" s="133">
         <f>AU41+AV41</f>
         <v>0</v>
       </c>
@@ -4827,42 +4840,42 @@
       <c r="J43" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120"/>
-      <c r="O43" s="120"/>
-      <c r="P43" s="120"/>
-      <c r="Q43" s="120"/>
-      <c r="R43" s="120"/>
-      <c r="S43" s="120"/>
-      <c r="T43" s="120"/>
-      <c r="U43" s="120"/>
-      <c r="V43" s="120"/>
-      <c r="W43" s="120"/>
-      <c r="X43" s="120"/>
-      <c r="Y43" s="120"/>
-      <c r="Z43" s="120"/>
-      <c r="AA43" s="120"/>
-      <c r="AB43" s="120"/>
-      <c r="AC43" s="120"/>
-      <c r="AD43" s="120"/>
-      <c r="AE43" s="120"/>
-      <c r="AF43" s="120"/>
-      <c r="AG43" s="120"/>
-      <c r="AH43" s="120"/>
-      <c r="AI43" s="120"/>
-      <c r="AJ43" s="120"/>
-      <c r="AK43" s="120"/>
-      <c r="AL43" s="120"/>
-      <c r="AM43" s="120"/>
-      <c r="AN43" s="120"/>
-      <c r="AO43" s="120"/>
-      <c r="AP43" s="120"/>
-      <c r="AQ43" s="120"/>
-      <c r="AR43" s="120"/>
-      <c r="AS43" s="120"/>
-      <c r="AT43" s="120"/>
+      <c r="K43" s="118"/>
+      <c r="L43" s="118"/>
+      <c r="M43" s="118"/>
+      <c r="N43" s="118"/>
+      <c r="O43" s="118"/>
+      <c r="P43" s="118"/>
+      <c r="Q43" s="118"/>
+      <c r="R43" s="118"/>
+      <c r="S43" s="118"/>
+      <c r="T43" s="118"/>
+      <c r="U43" s="118"/>
+      <c r="V43" s="118"/>
+      <c r="W43" s="118"/>
+      <c r="X43" s="118"/>
+      <c r="Y43" s="118"/>
+      <c r="Z43" s="118"/>
+      <c r="AA43" s="118"/>
+      <c r="AB43" s="118"/>
+      <c r="AC43" s="118"/>
+      <c r="AD43" s="118"/>
+      <c r="AE43" s="118"/>
+      <c r="AF43" s="118"/>
+      <c r="AG43" s="118"/>
+      <c r="AH43" s="118"/>
+      <c r="AI43" s="118"/>
+      <c r="AJ43" s="118"/>
+      <c r="AK43" s="118"/>
+      <c r="AL43" s="118"/>
+      <c r="AM43" s="118"/>
+      <c r="AN43" s="118"/>
+      <c r="AO43" s="118"/>
+      <c r="AP43" s="118"/>
+      <c r="AQ43" s="118"/>
+      <c r="AR43" s="118"/>
+      <c r="AS43" s="118"/>
+      <c r="AT43" s="118"/>
       <c r="AU43" s="112"/>
       <c r="AV43" s="112"/>
       <c r="AW43" s="105"/>
@@ -4922,18 +4935,19 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="R2:R6"/>
-    <mergeCell ref="S2:S6"/>
-    <mergeCell ref="AT2:AT6"/>
-    <mergeCell ref="AO2:AO6"/>
-    <mergeCell ref="AP2:AP6"/>
-    <mergeCell ref="AQ2:AQ6"/>
-    <mergeCell ref="AR2:AR6"/>
-    <mergeCell ref="AS2:AS6"/>
-    <mergeCell ref="AK2:AK6"/>
-    <mergeCell ref="AL2:AL6"/>
-    <mergeCell ref="AM2:AM6"/>
-    <mergeCell ref="AN2:AN6"/>
+    <mergeCell ref="AW12:AX12"/>
+    <mergeCell ref="AC2:AC6"/>
+    <mergeCell ref="AD2:AD6"/>
+    <mergeCell ref="AE2:AE6"/>
+    <mergeCell ref="Y2:Y6"/>
+    <mergeCell ref="Z2:Z6"/>
+    <mergeCell ref="AA2:AA6"/>
+    <mergeCell ref="AB2:AB6"/>
+    <mergeCell ref="AG2:AG6"/>
+    <mergeCell ref="AH2:AH6"/>
+    <mergeCell ref="AI2:AI6"/>
+    <mergeCell ref="AJ2:AJ6"/>
+    <mergeCell ref="AU3:AX3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="K2:K6"/>
     <mergeCell ref="L2:L6"/>
@@ -4950,19 +4964,18 @@
     <mergeCell ref="Q2:Q6"/>
     <mergeCell ref="T2:T6"/>
     <mergeCell ref="U2:U6"/>
-    <mergeCell ref="AW12:AX12"/>
-    <mergeCell ref="AC2:AC6"/>
-    <mergeCell ref="AD2:AD6"/>
-    <mergeCell ref="AE2:AE6"/>
-    <mergeCell ref="Y2:Y6"/>
-    <mergeCell ref="Z2:Z6"/>
-    <mergeCell ref="AA2:AA6"/>
-    <mergeCell ref="AB2:AB6"/>
-    <mergeCell ref="AG2:AG6"/>
-    <mergeCell ref="AH2:AH6"/>
-    <mergeCell ref="AI2:AI6"/>
-    <mergeCell ref="AJ2:AJ6"/>
-    <mergeCell ref="AU3:AX3"/>
+    <mergeCell ref="R2:R6"/>
+    <mergeCell ref="S2:S6"/>
+    <mergeCell ref="AT2:AT6"/>
+    <mergeCell ref="AO2:AO6"/>
+    <mergeCell ref="AP2:AP6"/>
+    <mergeCell ref="AQ2:AQ6"/>
+    <mergeCell ref="AR2:AR6"/>
+    <mergeCell ref="AS2:AS6"/>
+    <mergeCell ref="AK2:AK6"/>
+    <mergeCell ref="AL2:AL6"/>
+    <mergeCell ref="AM2:AM6"/>
+    <mergeCell ref="AN2:AN6"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>